<commit_message>
match to refactored version
</commit_message>
<xml_diff>
--- a/data/verification/gene_prioritization_runtime_memory.xlsx
+++ b/data/verification/gene_prioritization_runtime_memory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16780" yWindow="1480" windowWidth="29120" windowHeight="28220" tabRatio="500"/>
+    <workbookView xWindow="18000" yWindow="460" windowWidth="29120" windowHeight="28220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -570,7 +570,7 @@
   <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="198" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,7 +714,7 @@
       </c>
       <c r="B14" s="8">
         <f>SUM(B13*(E68+E81)+(E35+C38))</f>
-        <v>1531.6705750000006</v>
+        <v>1386.2957190000002</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -733,249 +733,249 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
+        <v>363</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="6">
+        <f>(B11*B3*2 +B11*B6)/B2</f>
+        <v>71.082864000000001</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17:E34" si="0">C17*D17</f>
+        <v>71.082864000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>364</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="6">
+        <f>B12*B3/B2</f>
+        <v>0.124712</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>364</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="6">
+        <f>B12*B3/B2</f>
+        <v>0.124712</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>365</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="6">
+        <f>B12*B3/B2</f>
+        <v>0.124712</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>369</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="6">
+        <f>(B12*C12*B4)/B2</f>
+        <v>0.93533999999999995</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0.93533999999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>371</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="6">
+        <f>C17</f>
+        <v>71.082864000000001</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>71.082864000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>372</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="6">
+        <f>C17</f>
+        <v>71.082864000000001</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>71.082864000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>374</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="6">
+        <f>C17*2</f>
+        <v>142.165728</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>142.165728</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>374</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="6">
+        <f>(B12*B7+B11*B7+B11*B6)/B2</f>
+        <v>35.603788000000002</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>35.603788000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>378</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="6">
+        <f>C25</f>
+        <v>35.603788000000002</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>35.603788000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>359</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="6">
+      <c r="B27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="6">
         <f>(B9*B8*B6+B9*B3+B8*B3)/B2</f>
         <v>9.8391999999999993E-2</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <f>C17*D17</f>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f>C27*D27</f>
         <v>9.8391999999999993E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>360</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C28" s="6">
         <f>(B10*B9*B6+B10*B3+B9*B3)/B2</f>
         <v>74.291991999999993</v>
       </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18">
-        <f t="shared" ref="E18:E34" si="0">C18*D18</f>
-        <v>148.58398399999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <f>C28*D28</f>
+        <v>74.291991999999993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>361</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C29" s="6">
         <f>B10*B3/B2</f>
         <v>0.15099199999999999</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <f>C29*D29</f>
         <v>0.15099199999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>363</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="6">
-        <f>(B11*B3*2 +B11*B6)/B2</f>
-        <v>71.082864000000001</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>142.165728</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>364</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="6">
-        <f>B12*B3/B2</f>
-        <v>0.124712</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>0.124712</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>364</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="6">
-        <f>B12*B3/B2</f>
-        <v>0.124712</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>0.124712</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>365</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="6">
-        <f>B12*B3/B2</f>
-        <v>0.124712</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>0.124712</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>369</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="6">
-        <f>(B12*C12*B4)/B2</f>
-        <v>0.93533999999999995</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>0.93533999999999995</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>371</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="6">
-        <f>C20</f>
-        <v>71.082864000000001</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>71.082864000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>372</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="6">
-        <f>C20</f>
-        <v>71.082864000000001</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>71.082864000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>374</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="6">
-        <f>C20*2</f>
-        <v>142.165728</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>142.165728</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>374</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="6">
-        <f>(B12*B7+B11*B7+B11*B6)/B2</f>
-        <v>35.603788000000002</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>35.603788000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>378</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="6">
-        <f>C28</f>
-        <v>35.603788000000002</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>35.603788000000002</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1081,7 +1081,7 @@
       <c r="D35"/>
       <c r="E35">
         <f>SUM(E17:E34)</f>
-        <v>893.73881200000017</v>
+        <v>748.36395600000003</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1103,7 +1103,7 @@
         <v>47</v>
       </c>
       <c r="C38" s="6">
-        <f>C34+C33+C32+C31+C29+C19</f>
+        <f>C34+C33+C32+C31+C26+C29</f>
         <v>97.464828000000011</v>
       </c>
       <c r="D38">
@@ -1141,7 +1141,7 @@
         <v>15</v>
       </c>
       <c r="C40" s="6">
-        <f>C29</f>
+        <f>C26</f>
         <v>35.603788000000002</v>
       </c>
       <c r="D40">
@@ -1691,7 +1691,7 @@
         <v>48</v>
       </c>
       <c r="C71" s="6">
-        <f>C19+C23</f>
+        <f>C29+C20</f>
         <v>0.275704</v>
       </c>
       <c r="D71" s="1">

</xml_diff>

<commit_message>
linked to production version
</commit_message>
<xml_diff>
--- a/data/verification/gene_prioritization_runtime_memory.xlsx
+++ b/data/verification/gene_prioritization_runtime_memory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10500" yWindow="460" windowWidth="28200" windowHeight="28220" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="28200" windowHeight="28220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,6 @@
     <t>Variable name</t>
   </si>
   <si>
-    <t>Input Variables</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
@@ -222,6 +219,9 @@
   </si>
   <si>
     <t>MB</t>
+  </si>
+  <si>
+    <t>bootstrap net Input Variables</t>
   </si>
 </sst>
 </file>
@@ -292,11 +292,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -345,8 +346,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="198" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="198" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,21 +644,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="C2" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -668,40 +670,40 @@
         <v>1000000</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <v>8</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -712,7 +714,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -723,7 +725,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -734,18 +736,18 @@
         <v>8</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -756,7 +758,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -767,7 +769,7 @@
         <v>491</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -778,7 +780,7 @@
         <v>18874</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -789,7 +791,7 @@
         <v>2961786</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -800,47 +802,47 @@
         <v>15589</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="8">
         <f>SUM(B16*(E71+E84)+(E38+C41))</f>
         <v>1386.5284490000004</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -924,7 +926,7 @@
         <v>369</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="14">
         <f>(B15*B6*B7)/B3</f>
@@ -1187,7 +1189,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B38" s="4"/>
       <c r="E38" s="12">
@@ -1200,16 +1202,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="C41" s="14">
         <f>C37+C36+C35+C34+C29+C32</f>
@@ -1225,7 +1227,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>19</v>
@@ -1244,7 +1246,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>15</v>
@@ -1266,7 +1268,7 @@
         <v>453</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C44" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1285,7 +1287,7 @@
         <v>454</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C45" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1304,7 +1306,7 @@
         <v>455</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C46" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1380,7 +1382,7 @@
         <v>461</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C50" s="14">
         <f>(B15  *B12  * B9)/B3</f>
@@ -1399,7 +1401,7 @@
         <v>463</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C51" s="14">
         <f>(B15* B9/B3)</f>
@@ -1418,7 +1420,7 @@
         <v>466</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C52" s="14">
         <f>(B15  ) *B12  * B9/B3</f>
@@ -1437,7 +1439,7 @@
         <v>466</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C53" s="14">
         <f>B12 * B8 /B3</f>
@@ -1456,7 +1458,7 @@
         <v>470</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C54" s="14">
         <f>B12 * B9/B3</f>
@@ -1475,7 +1477,7 @@
         <v>471</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C55" s="16">
         <f>B12*B9/B3</f>
@@ -1494,7 +1496,7 @@
         <v>472</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C56" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1513,7 +1515,7 @@
         <v>473</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C57" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1532,7 +1534,7 @@
         <v>475</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C58" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1551,7 +1553,7 @@
         <v>475</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C59" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1570,7 +1572,7 @@
         <v>477</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C60" s="16">
         <f>(B15 *  B9 /B3)</f>
@@ -1589,7 +1591,7 @@
         <v>478</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C61" s="16">
         <f>(B15 *  B9 /B3)</f>
@@ -1608,7 +1610,7 @@
         <v>479</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C62" s="16">
         <f>(B15 *  B9 /B3)</f>
@@ -1627,7 +1629,7 @@
         <v>481</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C63" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1646,7 +1648,7 @@
         <v>482</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C64" s="16">
         <f>(B15 *  B9 /B3)</f>
@@ -1665,7 +1667,7 @@
         <v>483</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C65" s="16">
         <f>(B15 *  B9 /B3)</f>
@@ -1684,7 +1686,7 @@
         <v>485</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C66" s="16">
         <f>(B15 *  B9 /B3)</f>
@@ -1703,7 +1705,7 @@
         <v>486</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C67" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1722,7 +1724,7 @@
         <v>487</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C68" s="16">
         <f>(B15 *  B9 /B3)</f>
@@ -1741,7 +1743,7 @@
         <v>488</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C69" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1760,7 +1762,7 @@
         <v>489</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C70" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1776,7 +1778,7 @@
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B71" s="4"/>
       <c r="E71" s="12">
@@ -1789,12 +1791,12 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C74" s="14">
         <f>C32+C23</f>
@@ -1813,7 +1815,7 @@
         <v>508</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C75" s="14">
         <f>B15 * B8 /B3</f>
@@ -1832,7 +1834,7 @@
         <v>509</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C76" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1851,7 +1853,7 @@
         <v>510</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C77" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1870,7 +1872,7 @@
         <v>511</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C78" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1889,7 +1891,7 @@
         <v>512</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C79" s="14">
         <f>(B15 *  B7 /B3)</f>
@@ -1908,7 +1910,7 @@
         <v>513</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C80" s="14">
         <f>(B15 *  B9 /B3)</f>
@@ -1927,7 +1929,7 @@
         <v>514</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C81" s="14">
         <f>B15 * B7/B3</f>
@@ -1946,7 +1948,7 @@
         <v>516</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C82" s="14">
         <f>6*B15*B9/B3</f>
@@ -1965,7 +1967,7 @@
         <v>521</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C83" s="14">
         <f>C82</f>
@@ -1981,7 +1983,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B84" s="4"/>
       <c r="E84" s="12">

</xml_diff>

<commit_message>
Update spreadsheet to have statistics for all major functions
</commit_message>
<xml_diff>
--- a/data/verification/gene_prioritization_runtime_memory.xlsx
+++ b/data/verification/gene_prioritization_runtime_memory.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lanier4/PycharmProjects/Gene_Prioritization_Pipeline/data/verification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingge2/PycharmProjects/KnowEng/dev/Gene_Prioritization_Pipeline/data/verification/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="27780" windowHeight="28220" tabRatio="500"/>
+    <workbookView xWindow="2520" yWindow="460" windowWidth="27680" windowHeight="16120" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="correlation" sheetId="2" r:id="rId1"/>
+    <sheet name="net_correlation" sheetId="3" r:id="rId2"/>
+    <sheet name="bootstrap_net_correlation" sheetId="1" r:id="rId3"/>
+    <sheet name="bootstrap_correlation" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="99">
   <si>
     <t>drug_response_df</t>
   </si>
@@ -222,6 +225,108 @@
   </si>
   <si>
     <t>(end bootstraps loop) 482</t>
+  </si>
+  <si>
+    <t>Input Variables</t>
+  </si>
+  <si>
+    <t>Byte</t>
+  </si>
+  <si>
+    <t>pandas df string</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Line number</t>
+  </si>
+  <si>
+    <t>Size/MB</t>
+  </si>
+  <si>
+    <t>drug_response_df_0</t>
+  </si>
+  <si>
+    <t>spreadsheet_df_0</t>
+  </si>
+  <si>
+    <t>consolodated_df</t>
+  </si>
+  <si>
+    <t>Total sum</t>
+  </si>
+  <si>
+    <t>parallel worker</t>
+  </si>
+  <si>
+    <t>Line number</t>
+  </si>
+  <si>
+    <t>df_header</t>
+  </si>
+  <si>
+    <t>result_df.index</t>
+  </si>
+  <si>
+    <t>intersection genes between original gene and net_genes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean </t>
+  </si>
+  <si>
+    <t>output column number</t>
+  </si>
+  <si>
+    <t>MByte</t>
+  </si>
+  <si>
+    <t>run_net_correlation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total sum </t>
+  </si>
+  <si>
+    <t>worker_for_run_net_correlation</t>
+  </si>
+  <si>
+    <t>name_size</t>
+  </si>
+  <si>
+    <t>samples not null</t>
+  </si>
+  <si>
+    <t>python empty list base size</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>number_of_bootstrap</t>
+  </si>
+  <si>
+    <t>run_bootstrap_correlation</t>
+  </si>
+  <si>
+    <t>worker_for_run_bootstrap_correlation outside</t>
+  </si>
+  <si>
+    <t>pcc_gm_array</t>
+  </si>
+  <si>
+    <t>worker_for_run_bootstrap_correlation inside</t>
+  </si>
+  <si>
+    <t>generate_bootstrap_coorelation_output</t>
   </si>
 </sst>
 </file>
@@ -231,7 +336,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -261,6 +366,48 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF008080"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Menlo Regular"/>
     </font>
   </fonts>
   <fills count="4">
@@ -299,7 +446,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -345,6 +492,21 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -626,9 +788,1229 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <f>1000000</f>
+        <v>1000000</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>491</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>18874</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>2961786</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>15589</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="8">
+        <f>C23+C30+C39</f>
+        <v>224.58701166666665</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>81</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="1">
+        <f>(B9*B8*B6+B9*B3+B8*B3)/B2</f>
+        <v>9.8391999999999993E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>82</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="1">
+        <f>(B10*B9*B6+B10*B3+B9*B3)/B2</f>
+        <v>74.291991999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>84</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1">
+        <f>B10*B4/B2</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>84</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1">
+        <f>B8*B4/B2</f>
+        <v>1.92E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>84</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="1">
+        <f>C18+C19</f>
+        <v>74.390383999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="21">
+        <f>SUM(C18:C22)</f>
+        <v>148.931952</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>127</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f>C18/24</f>
+        <v>4.0996666666666664E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <v>127</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <f>C19</f>
+        <v>74.291991999999993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>128</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <f>B10*B6/B2</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="19">
+        <f>SUM(C27:C29)</f>
+        <v>74.447083666666657</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <v>148</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <f>B10*B4/B2</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>149</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35">
+        <f>(B3*2+B6*3) * B10/B2</f>
+        <v>0.75495999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <v>152</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36">
+        <f>B4*5/B2</f>
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>153</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37">
+        <f>C34</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
+        <v>154</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38">
+        <f>C20</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
+      <c r="B39" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="19">
+        <f>SUM(C34:C38)</f>
+        <v>1.2079759999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <f>1000000</f>
+        <v>1000000</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>491</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>18874</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>2961786</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>15589</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13">
+        <v>13410</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="8">
+        <f>SUM(C31+C40) + B16*(C59+C74)</f>
+        <v>616.59492141666647</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>267</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f>(B9*B6/B2)</f>
+        <v>3.9280000000000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>268</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <f>(B10*B9*B6+B10*B3+B9*B3)/B2</f>
+        <v>74.291991999999993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <v>269</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <f>150992/B2</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <v>271</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <f>B11*3*B6/B2</f>
+        <v>71.082864000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>272</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <f>(B4*B12)/B2</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
+        <v>272</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <f>(B4*B12)/B2</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>273</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <f>(B4*B12)/B2</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <v>275</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <f>(B4*B12)/B2</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>277</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29">
+        <f>786528/B2</f>
+        <v>0.786528</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>279</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <f>B11*B6*3/B2</f>
+        <v>71.082864000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <v>280</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <f>B11*B6*3/B2</f>
+        <v>71.082864000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <v>282</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <f>C30+C31</f>
+        <v>142.165728</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>283</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <f>B11*2*3*B6/B2</f>
+        <v>142.165728</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <v>286</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <f>C33</f>
+        <v>142.165728</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>288</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35">
+        <f>(B12*B6/B2)</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <v>289</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36">
+        <f>C35</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>291</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
+        <f>18874/B2</f>
+        <v>1.8873999999999998E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
+        <v>291</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <f>(64+B8*8)/B2</f>
+        <v>7.2000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
+        <v>291</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39">
+        <f>((B10+B8)*B9*B6+(B10+B8)*B3+B9*B3)/B2</f>
+        <v>74.295928000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B40" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40">
+        <f>SUM(C33:C39)</f>
+        <v>358.89575399999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="6">
+        <v>327</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <f>C37/24</f>
+        <v>7.864166666666666E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="6">
+        <v>327</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <f>(B12*B9*B6+B12*B3+B9*B3)/B2</f>
+        <v>61.362231999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>329</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <f>C46</f>
+        <v>61.362231999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="6">
+        <v>333</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48">
+        <f>B12*B9*B6/B2</f>
+        <v>61.233592000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="6">
+        <v>335</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <f>B12*B6/B2</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="6">
+        <v>336</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50">
+        <f>C49</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
+        <v>337</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51">
+        <f>(B12 *  B6 /B2)</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="6">
+        <v>338</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52">
+        <f>(B12 *  B6 /B2)</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="6">
+        <v>339</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53">
+        <f>(B12 *  B6 /B2)</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="6">
+        <v>340</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54">
+        <f>(B12 *  B6 /B2)</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="6">
+        <v>342</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55">
+        <f>(B12 *  B6 /B2)</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="6">
+        <v>343</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56">
+        <f>(B12 *  B6 /B2)</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="6">
+        <v>345</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57">
+        <f>(B12 *  B6 /B2)</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="6">
+        <v>346</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58">
+        <f>(B12 *  B6 /B2)</f>
+        <v>0.124712</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B59" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59">
+        <f>SUM(C45:C58)</f>
+        <v>185.20596241666652</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="6">
+        <v>505</v>
+      </c>
+      <c r="B64" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64">
+        <f>B12*B14/B2</f>
+        <v>1.5589E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="6">
+        <v>506</v>
+      </c>
+      <c r="B65" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65">
+        <f>B13*B5/B2</f>
+        <v>0.10728</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="6">
+        <v>507</v>
+      </c>
+      <c r="B66" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66">
+        <f>B13*B5/B2</f>
+        <v>0.10728</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="6">
+        <v>508</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67">
+        <f>B13*B5/B2</f>
+        <v>0.10728</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="6">
+        <v>509</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C68">
+        <f>B13*B4/B2</f>
+        <v>0.10728</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="6">
+        <v>510</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69">
+        <f>B13*B6/B2</f>
+        <v>0.10728</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="6">
+        <v>511</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C70">
+        <f>B13*B4/B2</f>
+        <v>0.10728</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="6">
+        <v>513</v>
+      </c>
+      <c r="B71" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C71">
+        <f>B13*B14*B6/B2</f>
+        <v>0.10728</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="6">
+        <v>516</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C72">
+        <f>112/B2</f>
+        <v>1.12E-4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="6">
+        <v>518</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C73">
+        <f>B13*B15*B6/B2</f>
+        <v>0.64368000000000003</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B74" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74">
+        <f>SUM(C64:C73)</f>
+        <v>1.4103410000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="198" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1957,4 +3339,640 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C62"/>
+  <sheetViews>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <f>1000000</f>
+        <v>1000000</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>491</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10">
+        <v>442</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>18874</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>2961786</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>15589</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14">
+        <v>13410</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15">
+        <v>64</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="8">
+        <f>C30+B19*(C52+C41+C62)</f>
+        <v>561.30454600000007</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>162</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f>(B9*B8*B6+B9*B3+B8*B3)/B2</f>
+        <v>7.8639999999999995E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
+        <v>163</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <f>(B11*B9*B6+B11*B3+B9*B3)/B2</f>
+        <v>74.291991999999993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>165</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27">
+        <f>(B15+B11*B4)/B2</f>
+        <v>0.151056</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <v>165</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <f>(B15+B8*B4)/B2</f>
+        <v>7.2000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>165</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <f>(B8+B11)*B9*B6/B2</f>
+        <v>74.141000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30">
+        <f>SUM(C25:C29)</f>
+        <v>148.591984</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <v>215</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <f>(B9*B8*B6+B9*B3+B8*B3)/B2</f>
+        <v>7.8639999999999995E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>215</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <f>(B11*B9*B6+B11*B3+B9*B3)/B2</f>
+        <v>74.291991999999993</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <v>216</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36">
+        <f>B11*B6/B2</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>217</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37">
+        <f>B11*B6/B2</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
+        <v>218</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38">
+        <f>B11*B6/B2</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
+        <v>267</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39">
+        <f>B11*B6/B2</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="6">
+        <v>270</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40">
+        <f>B11*B6/B2</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="6"/>
+      <c r="B41" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41">
+        <f>SUM(C34:C40)</f>
+        <v>75.054816000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="6"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="24"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="6">
+        <v>220</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45">
+        <f>B11*B10*B6/B2</f>
+        <v>66.738463999999993</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="6">
+        <v>220</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46">
+        <f>B10*B8/B2</f>
+        <v>4.4200000000000001E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>223</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47">
+        <f>B9*B6/B2</f>
+        <v>3.9280000000000001E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="6">
+        <v>224</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48">
+        <f>B10*B6/B2</f>
+        <v>3.5360000000000001E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="6">
+        <v>225</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <f>B11*B6/B2</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="6">
+        <v>226</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50">
+        <f>B11*B6/B2</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
+        <v>227</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51">
+        <f>B11*B6/B2</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B52" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52">
+        <f xml:space="preserve"> SUM(C45:C51)*B17</f>
+        <v>335.99673000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="24"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="6">
+        <v>246</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57">
+        <f>B11*B4/B2</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="6">
+        <v>247</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C58">
+        <f>B11*B18*B6/B2</f>
+        <v>0.75495999999999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="6">
+        <v>250</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59">
+        <f>(B15+B18*B4)/B2</f>
+        <v>1.0399999999999999E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="6">
+        <v>251</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60">
+        <f>B11*B18*B6/B2</f>
+        <v>0.75495999999999996</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="6">
+        <v>252</v>
+      </c>
+      <c r="B61" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61">
+        <f>C57</f>
+        <v>0.15099199999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B62" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C62">
+        <f xml:space="preserve"> SUM(C57:C60)</f>
+        <v>1.661016</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>